<commit_message>
deze commit had al veel eerder moeten gebeuren
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laicoz\Documents\School\Periode 3.4\Artificial Intelligence\Sudoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CFC3AC-1CFF-4D10-BB5B-95FD01137C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14FF770-9458-435D-B4F9-629D836C0B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CB80FD01-812E-46F0-B64B-129F87E3FDC5}"/>
+    <workbookView xWindow="7200" yWindow="1245" windowWidth="21600" windowHeight="11385" xr2:uid="{CB80FD01-812E-46F0-B64B-129F87E3FDC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>x%9 = 1</t>
   </si>
@@ -49,6 +49,18 @@
   </si>
   <si>
     <t>x / 9</t>
+  </si>
+  <si>
+    <t>Forward</t>
+  </si>
+  <si>
+    <t>Backward</t>
+  </si>
+  <si>
+    <t>0; 24</t>
+  </si>
+  <si>
+    <t>00;02</t>
   </si>
 </sst>
 </file>
@@ -150,7 +162,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -159,6 +171,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Controlecel" xfId="1" builtinId="23"/>
@@ -475,13 +488,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B7B5A6-71DE-46D8-9197-A96F0C941567}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18:I20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
@@ -1102,6 +1118,47 @@
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="8">
+        <v>4.8611111111111112E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26" s="8">
+        <v>0.10069444444444443</v>
+      </c>
+      <c r="C26" s="8">
+        <v>0.93055555555555547</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="8">
+        <v>0.30694444444444441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>